<commit_message>
t/etc/align: test transcript B for Q96S55.fa alignments.
</commit_message>
<xml_diff>
--- a/t/etc/align/structure.xlsx
+++ b/t/etc/align/structure.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="-420" windowWidth="34400" windowHeight="22600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35560" windowHeight="20980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <definedName name="test_exons" localSheetId="0">Sheet1!$A$1:$H$31</definedName>
     <definedName name="test.clone.vulgar" localSheetId="0">Sheet1!$A$44:$CS$45</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Connection1" type="6" refreshedVersion="0">
+  <connection id="1" name="Connection1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:mg13:Work:Misc:Vulgar:RP11-420G6.2-002:test_exons.txt" tab="0" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
@@ -38,7 +38,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Connection2" type="6" refreshedVersion="0">
+  <connection id="2" name="Connection2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="6" sourceFile="Macintosh HD:Users:mg13:Work:Misc:Vulgar:RP11-420G6.2-002:test.clone.vulgar" tab="0" space="1" consecutive="1">
       <textFields count="97">
         <textField/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="128">
   <si>
     <t>Intron 4.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -462,19 +462,166 @@
   <si>
     <t>Intron 4.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sp|Q96S55|WRIP1_HUMAN</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Exon 1.1</t>
+  </si>
+  <si>
+    <t>Intron 1.1</t>
+  </si>
+  <si>
+    <t>Intron 1.2</t>
+  </si>
+  <si>
+    <t>Intron 1.3</t>
+  </si>
+  <si>
+    <t>Exon 2.1</t>
+  </si>
+  <si>
+    <t>Exon 2.2</t>
+  </si>
+  <si>
+    <t>Exon 2.3</t>
+  </si>
+  <si>
+    <t>Intron 2.1</t>
+  </si>
+  <si>
+    <t>Intron 2.2</t>
+  </si>
+  <si>
+    <t>Intron 2.3</t>
+  </si>
+  <si>
+    <t>Exon 3.1</t>
+  </si>
+  <si>
+    <t>Exon 3.2</t>
+  </si>
+  <si>
+    <t>Exon 3.3</t>
+  </si>
+  <si>
+    <t>Exon 3.4</t>
+  </si>
+  <si>
+    <t>Exon 3.5</t>
+  </si>
+  <si>
+    <t>Intron 3.1</t>
+  </si>
+  <si>
+    <t>Intron 3.2</t>
+  </si>
+  <si>
+    <t>Intron 3.3</t>
+  </si>
+  <si>
+    <t>Exon 4.1</t>
+  </si>
+  <si>
+    <t>Exon 4.2</t>
+  </si>
+  <si>
+    <t>Exon 4.3</t>
+  </si>
+  <si>
+    <t>Intron 4.1</t>
+  </si>
+  <si>
+    <t>Intron 4.2</t>
+  </si>
+  <si>
+    <t>Intron 4.3</t>
+  </si>
+  <si>
+    <t>Exon 5.1</t>
+  </si>
+  <si>
+    <t>Exon 5.2</t>
+  </si>
+  <si>
+    <t>Exon 5.3</t>
+  </si>
+  <si>
+    <t>Intron 5.1</t>
+  </si>
+  <si>
+    <t>Intron 5.2</t>
+  </si>
+  <si>
+    <t>Intron 5.3</t>
+  </si>
+  <si>
+    <t>Exon 6.1</t>
+  </si>
+  <si>
+    <t>Exon 6.2</t>
+  </si>
+  <si>
+    <t>Intron 6.1</t>
+  </si>
+  <si>
+    <t>Intron 6.2</t>
+  </si>
+  <si>
+    <t>Intron 6.3</t>
+  </si>
+  <si>
+    <t>Exon 7.1</t>
+  </si>
+  <si>
+    <t>Exon 1</t>
+  </si>
+  <si>
+    <t>Exon 2</t>
+  </si>
+  <si>
+    <t>Exon 3</t>
+  </si>
+  <si>
+    <t>Alignment taken from protein.clone.vulgar:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -495,30 +642,185 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="77">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_exons" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test.clone.vulgar" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test.clone.vulgar" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_exons" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,14 +1142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:H40"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -2944,7 +3246,7 @@
         <v>37340</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
         <v>58</v>
       </c>
@@ -2965,7 +3267,7 @@
         <v>41483</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
         <v>48</v>
       </c>
@@ -2986,7 +3288,7 @@
         <v>50549</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
         <v>59</v>
       </c>
@@ -3007,7 +3309,7 @@
         <v>52054</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
         <v>60</v>
       </c>
@@ -3028,12 +3330,1278 @@
         <v>55274</v>
       </c>
     </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>665</v>
+      </c>
+      <c r="D91" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" t="s">
+        <v>17</v>
+      </c>
+      <c r="F91">
+        <v>120540</v>
+      </c>
+      <c r="G91">
+        <v>140196</v>
+      </c>
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93">
+        <v>274</v>
+      </c>
+      <c r="C93">
+        <v>822</v>
+      </c>
+      <c r="E93">
+        <f>B91+1</f>
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <f>E93+B93-1</f>
+        <v>274</v>
+      </c>
+      <c r="G93">
+        <f>F91+1</f>
+        <v>120541</v>
+      </c>
+      <c r="H93">
+        <f>G93+C93-1</f>
+        <v>121362</v>
+      </c>
+      <c r="I93" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="3">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <f>F93+1</f>
+        <v>275</v>
+      </c>
+      <c r="F94">
+        <f t="shared" ref="F94" si="12">E94+B94-1</f>
+        <v>274</v>
+      </c>
+      <c r="G94">
+        <f>H93+1</f>
+        <v>121363</v>
+      </c>
+      <c r="H94">
+        <f t="shared" ref="H94" si="13">G94+C94-1</f>
+        <v>121364</v>
+      </c>
+      <c r="I94" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>2242</v>
+      </c>
+      <c r="E95">
+        <f t="shared" ref="E95:E128" si="14">F94+1</f>
+        <v>275</v>
+      </c>
+      <c r="F95">
+        <f t="shared" ref="F95:F128" si="15">E95+B95-1</f>
+        <v>274</v>
+      </c>
+      <c r="G95">
+        <f t="shared" ref="G95:G128" si="16">H94+1</f>
+        <v>121365</v>
+      </c>
+      <c r="H95">
+        <f t="shared" ref="H95:H128" si="17">G95+C95-1</f>
+        <v>123606</v>
+      </c>
+      <c r="I95" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="3">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="14"/>
+        <v>275</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="15"/>
+        <v>274</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="16"/>
+        <v>123607</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="17"/>
+        <v>123608</v>
+      </c>
+      <c r="I96" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>33</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="14"/>
+        <v>275</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="15"/>
+        <v>285</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="16"/>
+        <v>123609</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="17"/>
+        <v>123641</v>
+      </c>
+      <c r="I97" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="14"/>
+        <v>286</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="15"/>
+        <v>285</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="16"/>
+        <v>123642</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="17"/>
+        <v>123642</v>
+      </c>
+      <c r="I98" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99">
+        <v>53</v>
+      </c>
+      <c r="C99">
+        <v>159</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="14"/>
+        <v>286</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="15"/>
+        <v>338</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="16"/>
+        <v>123643</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="17"/>
+        <v>123801</v>
+      </c>
+      <c r="I99" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="3">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="14"/>
+        <v>339</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="15"/>
+        <v>338</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="16"/>
+        <v>123802</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="17"/>
+        <v>123803</v>
+      </c>
+      <c r="I100" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>1233</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="14"/>
+        <v>339</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="15"/>
+        <v>338</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="16"/>
+        <v>123804</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="17"/>
+        <v>125036</v>
+      </c>
+      <c r="I101" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="2">
+        <v>3</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="14"/>
+        <v>339</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="15"/>
+        <v>338</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="16"/>
+        <v>125037</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="17"/>
+        <v>125038</v>
+      </c>
+      <c r="I102" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103">
+        <v>43</v>
+      </c>
+      <c r="C103">
+        <v>129</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="14"/>
+        <v>339</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="15"/>
+        <v>381</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="16"/>
+        <v>125039</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="17"/>
+        <v>125167</v>
+      </c>
+      <c r="I103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="14"/>
+        <v>382</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="15"/>
+        <v>381</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="16"/>
+        <v>125168</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="17"/>
+        <v>125168</v>
+      </c>
+      <c r="I104" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="14"/>
+        <v>382</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="15"/>
+        <v>382</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="16"/>
+        <v>125169</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="17"/>
+        <v>125168</v>
+      </c>
+      <c r="I105" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106">
+        <v>36</v>
+      </c>
+      <c r="C106">
+        <v>108</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="14"/>
+        <v>383</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="15"/>
+        <v>418</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="16"/>
+        <v>125169</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="17"/>
+        <v>125276</v>
+      </c>
+      <c r="I106" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="14"/>
+        <v>419</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="15"/>
+        <v>418</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="16"/>
+        <v>125277</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="17"/>
+        <v>125278</v>
+      </c>
+      <c r="I107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="2">
+        <v>5</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="14"/>
+        <v>419</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="15"/>
+        <v>418</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="16"/>
+        <v>125279</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="17"/>
+        <v>125280</v>
+      </c>
+      <c r="I108" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>8897</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="14"/>
+        <v>419</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="15"/>
+        <v>418</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="16"/>
+        <v>125281</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="17"/>
+        <v>134177</v>
+      </c>
+      <c r="I109" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="2">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="14"/>
+        <v>419</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="15"/>
+        <v>418</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="16"/>
+        <v>134178</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="17"/>
+        <v>134179</v>
+      </c>
+      <c r="I110" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="14"/>
+        <v>419</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="15"/>
+        <v>419</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="16"/>
+        <v>134180</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="17"/>
+        <v>134180</v>
+      </c>
+      <c r="I111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112">
+        <v>76</v>
+      </c>
+      <c r="C112">
+        <v>228</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="14"/>
+        <v>420</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="16"/>
+        <v>134181</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="17"/>
+        <v>134408</v>
+      </c>
+      <c r="I112" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="14"/>
+        <v>496</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="16"/>
+        <v>134409</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="17"/>
+        <v>134409</v>
+      </c>
+      <c r="I113" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" s="2">
+        <v>5</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="14"/>
+        <v>496</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="16"/>
+        <v>134410</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="17"/>
+        <v>134411</v>
+      </c>
+      <c r="I114" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>3909</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="14"/>
+        <v>496</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="16"/>
+        <v>134412</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="17"/>
+        <v>138320</v>
+      </c>
+      <c r="I115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" s="2">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="14"/>
+        <v>496</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="16"/>
+        <v>138321</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="17"/>
+        <v>138322</v>
+      </c>
+      <c r="I116" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="14"/>
+        <v>496</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="15"/>
+        <v>496</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="16"/>
+        <v>138323</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="17"/>
+        <v>138324</v>
+      </c>
+      <c r="I117" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118">
+        <v>51</v>
+      </c>
+      <c r="C118">
+        <v>153</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="14"/>
+        <v>497</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="16"/>
+        <v>138325</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="17"/>
+        <v>138477</v>
+      </c>
+      <c r="I118" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="14"/>
+        <v>548</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="16"/>
+        <v>138478</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="17"/>
+        <v>138478</v>
+      </c>
+      <c r="I119" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" s="2">
+        <v>5</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="14"/>
+        <v>548</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="16"/>
+        <v>138479</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="17"/>
+        <v>138480</v>
+      </c>
+      <c r="I120" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>758</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="14"/>
+        <v>548</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="16"/>
+        <v>138481</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="17"/>
+        <v>139238</v>
+      </c>
+      <c r="I121" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" s="2">
+        <v>3</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="14"/>
+        <v>548</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="16"/>
+        <v>139239</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="17"/>
+        <v>139240</v>
+      </c>
+      <c r="I122" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="14"/>
+        <v>548</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="15"/>
+        <v>548</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="16"/>
+        <v>139241</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="17"/>
+        <v>139242</v>
+      </c>
+      <c r="I123" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B124">
+        <v>26</v>
+      </c>
+      <c r="C124">
+        <v>78</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="14"/>
+        <v>549</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="15"/>
+        <v>574</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="16"/>
+        <v>139243</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="17"/>
+        <v>139320</v>
+      </c>
+      <c r="I124" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" s="2">
+        <v>5</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="14"/>
+        <v>575</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="15"/>
+        <v>574</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="16"/>
+        <v>139321</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="17"/>
+        <v>139322</v>
+      </c>
+      <c r="I125" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>599</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="14"/>
+        <v>575</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="15"/>
+        <v>574</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="16"/>
+        <v>139323</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="17"/>
+        <v>139921</v>
+      </c>
+      <c r="I126" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="2">
+        <v>3</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="14"/>
+        <v>575</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="15"/>
+        <v>574</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="16"/>
+        <v>139922</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="17"/>
+        <v>139923</v>
+      </c>
+      <c r="I127" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B128">
+        <v>91</v>
+      </c>
+      <c r="C128">
+        <v>273</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="14"/>
+        <v>575</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="15"/>
+        <v>665</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="16"/>
+        <v>139924</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="17"/>
+        <v>140196</v>
+      </c>
+      <c r="I128" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E131">
+        <f>E93</f>
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <f>F93</f>
+        <v>274</v>
+      </c>
+      <c r="G131">
+        <f>G93</f>
+        <v>120541</v>
+      </c>
+      <c r="H131">
+        <f>H93</f>
+        <v>121362</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E132">
+        <f>E97</f>
+        <v>275</v>
+      </c>
+      <c r="F132">
+        <f>F99</f>
+        <v>338</v>
+      </c>
+      <c r="G132">
+        <f>G97</f>
+        <v>123609</v>
+      </c>
+      <c r="H132">
+        <f>H99</f>
+        <v>123801</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E133">
+        <f>E103</f>
+        <v>339</v>
+      </c>
+      <c r="F133">
+        <f>F107</f>
+        <v>418</v>
+      </c>
+      <c r="G133">
+        <f>G103</f>
+        <v>125039</v>
+      </c>
+      <c r="H133">
+        <f>H107</f>
+        <v>125278</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E134">
+        <f>E111</f>
+        <v>419</v>
+      </c>
+      <c r="F134">
+        <f>F113</f>
+        <v>495</v>
+      </c>
+      <c r="G134">
+        <f>G111</f>
+        <v>134180</v>
+      </c>
+      <c r="H134">
+        <f>H113</f>
+        <v>134409</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E135">
+        <f>E117</f>
+        <v>496</v>
+      </c>
+      <c r="F135">
+        <f>F119</f>
+        <v>547</v>
+      </c>
+      <c r="G135">
+        <f>G117</f>
+        <v>138323</v>
+      </c>
+      <c r="H135">
+        <f>H119</f>
+        <v>138478</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E136">
+        <f>E123</f>
+        <v>548</v>
+      </c>
+      <c r="F136">
+        <f>F124</f>
+        <v>574</v>
+      </c>
+      <c r="G136">
+        <f>G123</f>
+        <v>139241</v>
+      </c>
+      <c r="H136">
+        <f>H124</f>
+        <v>139320</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E137">
+        <f>E128</f>
+        <v>575</v>
+      </c>
+      <c r="F137">
+        <f>F128</f>
+        <v>665</v>
+      </c>
+      <c r="G137">
+        <f>G128</f>
+        <v>139924</v>
+      </c>
+      <c r="H137">
+        <f>H128</f>
+        <v>140196</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>